<commit_message>
Pre Invoice No header
</commit_message>
<xml_diff>
--- a/Pre_Invoice_Template.xlsx
+++ b/Pre_Invoice_Template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Xavier/Desktop/HiPro_Invoicing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Xavier/Desktop/Billing_System/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F32F6274-53FD-224C-859E-65E38462043F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E5CA163-8367-204F-9597-17FBB506E51F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14240" tabRatio="858" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -697,6 +697,9 @@
     <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -723,9 +726,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1071,8 +1071,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:N281"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1126,9 +1126,9 @@
       <c r="A3" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="66"/>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
+      <c r="B3" s="57"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
       <c r="E3" s="40"/>
       <c r="F3" s="40"/>
       <c r="H3" s="54"/>
@@ -1145,11 +1145,11 @@
       <c r="D4" s="44"/>
       <c r="E4" s="41"/>
       <c r="F4" s="41"/>
-      <c r="G4" s="57" t="s">
+      <c r="G4" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="58"/>
-      <c r="I4" s="59"/>
+      <c r="H4" s="59"/>
+      <c r="I4" s="60"/>
       <c r="M4" s="6"/>
     </row>
     <row r="5" spans="1:14" ht="14" customHeight="1" x14ac:dyDescent="0.15">
@@ -1161,9 +1161,9 @@
       <c r="D5" s="47"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
-      <c r="G5" s="60"/>
-      <c r="H5" s="61"/>
-      <c r="I5" s="62"/>
+      <c r="G5" s="61"/>
+      <c r="H5" s="62"/>
+      <c r="I5" s="63"/>
       <c r="M5" s="6"/>
     </row>
     <row r="6" spans="1:14" ht="14" customHeight="1" x14ac:dyDescent="0.15">
@@ -1175,9 +1175,9 @@
       <c r="D6" s="44"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="60"/>
-      <c r="H6" s="61"/>
-      <c r="I6" s="62"/>
+      <c r="G6" s="61"/>
+      <c r="H6" s="62"/>
+      <c r="I6" s="63"/>
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
     </row>
@@ -1190,9 +1190,9 @@
       <c r="D7" s="44"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="60"/>
-      <c r="H7" s="61"/>
-      <c r="I7" s="62"/>
+      <c r="G7" s="61"/>
+      <c r="H7" s="62"/>
+      <c r="I7" s="63"/>
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
     </row>
@@ -1200,9 +1200,9 @@
       <c r="B8" s="29"/>
       <c r="C8" s="36"/>
       <c r="D8" s="37"/>
-      <c r="G8" s="60"/>
-      <c r="H8" s="61"/>
-      <c r="I8" s="62"/>
+      <c r="G8" s="61"/>
+      <c r="H8" s="62"/>
+      <c r="I8" s="63"/>
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
     </row>
@@ -1215,9 +1215,9 @@
       <c r="D9" s="56"/>
       <c r="E9" s="51"/>
       <c r="F9" s="51"/>
-      <c r="G9" s="60"/>
-      <c r="H9" s="61"/>
-      <c r="I9" s="62"/>
+      <c r="G9" s="61"/>
+      <c r="H9" s="62"/>
+      <c r="I9" s="63"/>
       <c r="L9" s="6"/>
       <c r="M9" s="6"/>
       <c r="N9" t="s">
@@ -1231,9 +1231,9 @@
       <c r="D10" s="56"/>
       <c r="E10" s="51"/>
       <c r="F10" s="51"/>
-      <c r="G10" s="60"/>
-      <c r="H10" s="61"/>
-      <c r="I10" s="62"/>
+      <c r="G10" s="61"/>
+      <c r="H10" s="62"/>
+      <c r="I10" s="63"/>
       <c r="L10" s="6"/>
       <c r="N10" t="s">
         <v>18</v>
@@ -1246,9 +1246,9 @@
       <c r="D11" s="56"/>
       <c r="E11" s="51"/>
       <c r="F11" s="51"/>
-      <c r="G11" s="60"/>
-      <c r="H11" s="61"/>
-      <c r="I11" s="62"/>
+      <c r="G11" s="61"/>
+      <c r="H11" s="62"/>
+      <c r="I11" s="63"/>
       <c r="L11" s="6"/>
     </row>
     <row r="12" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1258,9 +1258,9 @@
       <c r="D12" s="56"/>
       <c r="E12" s="51"/>
       <c r="F12" s="51"/>
-      <c r="G12" s="60"/>
-      <c r="H12" s="61"/>
-      <c r="I12" s="62"/>
+      <c r="G12" s="61"/>
+      <c r="H12" s="62"/>
+      <c r="I12" s="63"/>
       <c r="L12" s="6"/>
     </row>
     <row r="13" spans="1:14" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
@@ -1270,9 +1270,9 @@
       <c r="D13" s="56"/>
       <c r="E13" s="51"/>
       <c r="F13" s="51"/>
-      <c r="G13" s="63"/>
-      <c r="H13" s="64"/>
-      <c r="I13" s="65"/>
+      <c r="G13" s="64"/>
+      <c r="H13" s="65"/>
+      <c r="I13" s="66"/>
       <c r="L13" s="6"/>
     </row>
     <row r="14" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1666,7 +1666,7 @@
     <mergeCell ref="G4:I13"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
-  <dataValidations count="3">
+  <dataValidations disablePrompts="1" count="3">
     <dataValidation type="whole" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Quantity" error="You must enter a number in this cell." promptTitle="Quantity" sqref="B19:C21 A18:A21" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>0</formula1>
       <formula2>1000000000</formula2>
@@ -1680,9 +1680,7 @@
   <pageMargins left="0.5" right="0" top="1.5" bottom="0.5" header="0" footer="0.4"/>
   <pageSetup orientation="landscape" horizontalDpi="300"/>
   <headerFooter alignWithMargins="0">
-    <oddHeader>&amp;C&amp;G</oddHeader>
     <oddFooter>Page &amp;P</oddFooter>
   </headerFooter>
-  <legacyDrawingHF r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>